<commit_message>
New violins with jitter
</commit_message>
<xml_diff>
--- a/Stimuli_Exp1_subselection.xlsx
+++ b/Stimuli_Exp1_subselection.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1282,7 +1285,7 @@
     <t xml:space="preserve">buen</t>
   </si>
   <si>
-    <t xml:space="preserve">ternasco</t>
+    <t xml:space="preserve">cordero</t>
   </si>
   <si>
     <t xml:space="preserve">guisos</t>
@@ -1865,83 +1868,103 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCFCFC"/>
+          <bgColor rgb="FF1B1E20"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:V259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A219" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S263" activeCellId="0" sqref="S263"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K239" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O239" activeCellId="0" sqref="O239"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -17336,12 +17359,14 @@
       <c r="T259" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:S259"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.700694444444445" right="0.700694444444445" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code to generate unique elements within all the characters from the sentences stimuli. We got a new file as a result: tokens4SentenceStimuli.csv
</commit_message>
<xml_diff>
--- a/Stimuli_Exp1_subselection.xlsx
+++ b/Stimuli_Exp1_subselection.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1861,30 +1862,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCFCFC"/>
-          <bgColor rgb="FF1B1E20"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1893,26 +1877,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:V259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K239" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O239" activeCellId="0" sqref="O239"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L192" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q237" activeCellId="0" sqref="Q237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16334,7 +16322,7 @@
         <v>565</v>
       </c>
       <c r="S242" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T242" s="5"/>
     </row>
@@ -16394,7 +16382,7 @@
         <v>566</v>
       </c>
       <c r="S243" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T243" s="5"/>
     </row>
@@ -16454,7 +16442,7 @@
         <v>565</v>
       </c>
       <c r="S244" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T244" s="5"/>
     </row>
@@ -16514,7 +16502,7 @@
         <v>566</v>
       </c>
       <c r="S245" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T245" s="5"/>
     </row>
@@ -16574,7 +16562,7 @@
         <v>566</v>
       </c>
       <c r="S246" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T246" s="5"/>
     </row>
@@ -16634,7 +16622,7 @@
         <v>566</v>
       </c>
       <c r="S247" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T247" s="5"/>
     </row>
@@ -16694,7 +16682,7 @@
         <v>566</v>
       </c>
       <c r="S248" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T248" s="5"/>
     </row>
@@ -16754,7 +16742,7 @@
         <v>566</v>
       </c>
       <c r="S249" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T249" s="5"/>
     </row>
@@ -16814,7 +16802,7 @@
         <v>567</v>
       </c>
       <c r="S250" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T250" s="5"/>
     </row>
@@ -16874,7 +16862,7 @@
         <v>564</v>
       </c>
       <c r="S251" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T251" s="5"/>
     </row>
@@ -16934,7 +16922,7 @@
         <v>567</v>
       </c>
       <c r="S252" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T252" s="5"/>
     </row>
@@ -16994,7 +16982,7 @@
         <v>564</v>
       </c>
       <c r="S253" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T253" s="5"/>
     </row>
@@ -17054,7 +17042,7 @@
         <v>565</v>
       </c>
       <c r="S254" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T254" s="5"/>
     </row>
@@ -17114,7 +17102,7 @@
         <v>569</v>
       </c>
       <c r="S255" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T255" s="5"/>
     </row>
@@ -17174,7 +17162,7 @@
         <v>566</v>
       </c>
       <c r="S256" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T256" s="5"/>
     </row>
@@ -17234,7 +17222,7 @@
         <v>569</v>
       </c>
       <c r="S257" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T257" s="5"/>
     </row>
@@ -17294,7 +17282,7 @@
         <v>566</v>
       </c>
       <c r="S258" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T258" s="5"/>
     </row>
@@ -17354,15 +17342,15 @@
         <v>571</v>
       </c>
       <c r="S259" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T259" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:S259"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
typo fixed from digido to dirigido
</commit_message>
<xml_diff>
--- a/Stimuli_Exp1_subselection.xlsx
+++ b/Stimuli_Exp1_subselection.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1616,7 +1617,7 @@
     <t xml:space="preserve">sospechosa</t>
   </si>
   <si>
-    <t xml:space="preserve">digido</t>
+    <t xml:space="preserve">dirigido</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -1884,7 +1885,7 @@
   <dimension ref="A1:V259"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L192" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q237" activeCellId="0" sqref="Q237"/>
+      <selection pane="topLeft" activeCell="P225" activeCellId="0" sqref="P225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Output sequences for sentence level
</commit_message>
<xml_diff>
--- a/Stimuli_Exp1_subselection.xlsx
+++ b/Stimuli_Exp1_subselection.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$S$259</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3168" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="569">
   <si>
     <t xml:space="preserve">stimuli</t>
   </si>
@@ -1732,15 +1733,6 @@
   </si>
   <si>
     <t xml:space="preserve">xxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xxxxxxxxxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xxxxxxxxxxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -1882,10 +1874,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V259"/>
+  <dimension ref="A1:V251"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L192" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P225" activeCellId="0" sqref="P225"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A205" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D264" activeCellId="0" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16867,486 +16859,6 @@
       </c>
       <c r="T251" s="5"/>
     </row>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="0" t="n">
-        <v>251</v>
-      </c>
-      <c r="B252" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="C252" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D252" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E252" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F252" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G252" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H252" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I252" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J252" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K252" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L252" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M252" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N252" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="O252" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="P252" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="Q252" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="R252" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="S252" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T252" s="5"/>
-    </row>
-    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="0" t="n">
-        <v>252</v>
-      </c>
-      <c r="B253" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="C253" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D253" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E253" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F253" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G253" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H253" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I253" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J253" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K253" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L253" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M253" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N253" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="O253" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="P253" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="Q253" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="R253" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="S253" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T253" s="5"/>
-    </row>
-    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="0" t="n">
-        <v>253</v>
-      </c>
-      <c r="B254" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="C254" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D254" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E254" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F254" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G254" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H254" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I254" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J254" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K254" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L254" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M254" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N254" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="O254" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="P254" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="Q254" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="R254" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="S254" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T254" s="5"/>
-    </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="0" t="n">
-        <v>254</v>
-      </c>
-      <c r="B255" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="C255" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D255" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E255" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F255" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G255" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H255" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I255" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J255" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K255" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L255" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M255" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N255" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="O255" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="P255" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="Q255" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="R255" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="S255" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T255" s="5"/>
-    </row>
-    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="B256" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="C256" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D256" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E256" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F256" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G256" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H256" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I256" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J256" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K256" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L256" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M256" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N256" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="O256" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="P256" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="Q256" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="R256" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="S256" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T256" s="5"/>
-    </row>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="B257" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="C257" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D257" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E257" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F257" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G257" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H257" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I257" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J257" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K257" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L257" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M257" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N257" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="O257" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="P257" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="Q257" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="R257" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="S257" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T257" s="5"/>
-    </row>
-    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="0" t="n">
-        <v>257</v>
-      </c>
-      <c r="B258" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="C258" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D258" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E258" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F258" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G258" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H258" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I258" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J258" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K258" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L258" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M258" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N258" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="O258" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="P258" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="Q258" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="R258" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="S258" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T258" s="5"/>
-    </row>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0" t="n">
-        <v>258</v>
-      </c>
-      <c r="B259" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="C259" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="D259" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="E259" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="F259" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G259" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H259" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="I259" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J259" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K259" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="L259" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="M259" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="N259" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="O259" s="0" t="s">
-        <v>571</v>
-      </c>
-      <c r="P259" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="Q259" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="R259" s="0" t="s">
-        <v>571</v>
-      </c>
-      <c r="S259" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T259" s="5"/>
-    </row>
   </sheetData>
   <autoFilter ref="B1:S259"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>